<commit_message>
committing files related to Obligation Suite- Naveen Task
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Suite.xlsx
@@ -517,8 +517,8 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,14 +643,14 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>39</v>
+      <c r="C12" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,14 +720,14 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>31</v>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
commiting all files of suite Interpretations- Naveen Task
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Suite.xlsx
@@ -160,7 +160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,6 +170,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -210,6 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,7 +525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,14 +650,14 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>31</v>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,14 +694,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>39</v>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
committing reportNG jars and changes in testng.xml and purchaseOrder suite files
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Suite.xlsx
@@ -536,7 +536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>39</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>